<commit_message>
update PLM Iteration evaluation
</commit_message>
<xml_diff>
--- a/documentation/codeAnalysis/PLM-iteration1-evaluation.xlsx
+++ b/documentation/codeAnalysis/PLM-iteration1-evaluation.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="iteration1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="25">
   <si>
     <t>Registration Feature</t>
   </si>
@@ -132,25 +132,30 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Zapf Dingbats"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="8">
@@ -247,8 +252,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -276,33 +283,33 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="25">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -315,6 +322,7 @@
     <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -327,6 +335,7 @@
     <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -660,7 +669,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
+      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -673,237 +682,269 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33" customHeight="1" thickBot="1">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="17" thickBot="1">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="4"/>
-      <c r="H2" s="2" t="s">
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
-      <c r="K2" s="4"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="7"/>
     </row>
     <row r="3" spans="1:11" ht="32" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="7" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="7" t="s">
+      <c r="E3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="G3" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="H3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="7" t="s">
+      <c r="I3" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="8">
+      <c r="A4" s="2">
         <v>1</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="8">
+      <c r="C4" s="2">
         <f xml:space="preserve"> 136 + 46</f>
         <v>182</v>
       </c>
-      <c r="D4" s="8">
+      <c r="D4" s="2">
         <f xml:space="preserve"> 0 + 3</f>
         <v>3</v>
       </c>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8" t="s">
+      <c r="E4" s="2">
+        <v>16</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="8"/>
-      <c r="J4" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="8"/>
+      <c r="H4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="8">
+      <c r="A5" s="2">
         <v>2</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="8">
+      <c r="C5" s="2">
         <f xml:space="preserve"> 137 + 60</f>
         <v>197</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="2">
         <f xml:space="preserve"> 0 + 3</f>
         <v>3</v>
       </c>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8" t="s">
+      <c r="E5" s="2">
+        <v>14</v>
+      </c>
+      <c r="F5" s="2">
+        <v>0</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="8"/>
+      <c r="H5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="8">
+      <c r="A6" s="2">
         <v>3</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="8">
+      <c r="C6" s="2">
         <f xml:space="preserve"> 184 + 3</f>
         <v>187</v>
       </c>
-      <c r="D6" s="8">
+      <c r="D6" s="2">
         <f xml:space="preserve"> 0 + 1</f>
         <v>1</v>
       </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8" t="s">
+      <c r="E6" s="2">
+        <v>7</v>
+      </c>
+      <c r="F6" s="2">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="8"/>
-      <c r="J6" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="8"/>
+      <c r="H6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="2"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="8">
+      <c r="A7" s="2">
         <v>4</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="2">
         <f xml:space="preserve"> 137 +  225</f>
         <v>362</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="2">
         <f xml:space="preserve"> 0  + 5</f>
         <v>5</v>
       </c>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8" t="s">
+      <c r="E7" s="2">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2">
+        <v>0</v>
+      </c>
+      <c r="G7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="8"/>
+      <c r="H7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="2"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="8">
+      <c r="A8" s="2">
         <v>5</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="8">
+      <c r="C8" s="2">
         <f xml:space="preserve"> 149 + 239</f>
         <v>388</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="2">
         <f xml:space="preserve"> 0 + 8</f>
         <v>8</v>
       </c>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8" t="s">
+      <c r="E8" s="2">
+        <v>18</v>
+      </c>
+      <c r="F8" s="2">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="8"/>
-      <c r="J8" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K8" s="8"/>
+      <c r="H8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="2"/>
+      <c r="J8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="2"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="8">
+      <c r="A9" s="2">
         <v>6</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="K9" s="8"/>
+      <c r="C9" s="2">
+        <f xml:space="preserve"> 149 + 239</f>
+        <v>388</v>
+      </c>
+      <c r="D9" s="2">
+        <f xml:space="preserve"> 0 + 8</f>
+        <v>8</v>
+      </c>
+      <c r="E9" s="2">
+        <v>4</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="2"/>
+      <c r="J9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>

<commit_message>
update PLM Iteration1 evaluation
</commit_message>
<xml_diff>
--- a/documentation/codeAnalysis/PLM-iteration1-evaluation.xlsx
+++ b/documentation/codeAnalysis/PLM-iteration1-evaluation.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="iteration1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -283,15 +283,12 @@
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -302,11 +299,14 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="27">
@@ -669,7 +669,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F8" sqref="F8"/>
+      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -682,269 +682,281 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="33" customHeight="1" thickBot="1">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
     </row>
     <row r="2" spans="1:11" ht="17" thickBot="1">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="5" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="6"/>
+      <c r="H2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="7"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:11" ht="32" customHeight="1">
       <c r="A3" s="8"/>
       <c r="B3" s="8"/>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="9" t="s">
+      <c r="H3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="I3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="K3" s="9" t="s">
+      <c r="K3" s="3" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:11">
-      <c r="A4" s="2">
+      <c r="A4" s="1">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="2">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
         <f xml:space="preserve"> 136 + 46</f>
         <v>182</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="1">
         <f xml:space="preserve"> 0 + 3</f>
         <v>3</v>
       </c>
-      <c r="E4" s="2">
-        <v>16</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2" t="s">
+      <c r="E4" s="1">
+        <v>26</v>
+      </c>
+      <c r="F4" s="1">
+        <v>0</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="2"/>
-      <c r="J4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="2"/>
+      <c r="H4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="1">
+        <v>0</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11">
-      <c r="A5" s="2">
+      <c r="A5" s="1">
         <v>2</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5" s="1">
         <f xml:space="preserve"> 137 + 60</f>
         <v>197</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D5" s="1">
         <f xml:space="preserve"> 0 + 3</f>
         <v>3</v>
       </c>
-      <c r="E5" s="2">
-        <v>14</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2" t="s">
+      <c r="E5" s="1">
+        <v>24</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="2"/>
-      <c r="J5" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="2"/>
+      <c r="H5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="1">
+        <v>0</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="1"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="2">
+      <c r="A6" s="1">
         <v>3</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6" s="1">
         <f xml:space="preserve"> 184 + 3</f>
         <v>187</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D6" s="1">
         <f xml:space="preserve"> 0 + 1</f>
         <v>1</v>
       </c>
-      <c r="E6" s="2">
-        <v>7</v>
-      </c>
-      <c r="F6" s="2">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2" t="s">
+      <c r="E6" s="1">
+        <v>17</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="2"/>
-      <c r="J6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="2"/>
+      <c r="H6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11">
-      <c r="A7" s="2">
+      <c r="A7" s="1">
         <v>4</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7" s="1">
         <f xml:space="preserve"> 137 +  225</f>
         <v>362</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="1">
         <f xml:space="preserve"> 0  + 5</f>
         <v>5</v>
       </c>
-      <c r="E7" s="2">
-        <v>12</v>
-      </c>
-      <c r="F7" s="2">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2" t="s">
+      <c r="E7" s="1">
+        <v>22</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="2"/>
-      <c r="J7" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="1">
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="1"/>
     </row>
     <row r="8" spans="1:11">
-      <c r="A8" s="2">
+      <c r="A8" s="1">
         <v>5</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8" s="1">
         <f xml:space="preserve"> 149 + 239</f>
         <v>388</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="1">
         <f xml:space="preserve"> 0 + 8</f>
         <v>8</v>
       </c>
-      <c r="E8" s="2">
-        <v>18</v>
-      </c>
-      <c r="F8" s="2">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2" t="s">
+      <c r="E8" s="1">
+        <v>28</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="2"/>
-      <c r="J8" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K8" s="2"/>
+      <c r="H8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="1"/>
     </row>
     <row r="9" spans="1:11">
-      <c r="A9" s="2">
+      <c r="A9" s="1">
         <v>6</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9" s="1">
         <f xml:space="preserve"> 149 + 239</f>
         <v>388</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="1">
         <f xml:space="preserve"> 0 + 8</f>
         <v>8</v>
       </c>
-      <c r="E9" s="2">
-        <v>4</v>
-      </c>
-      <c r="F9" s="2">
-        <v>0</v>
-      </c>
-      <c r="G9" s="2" t="s">
+      <c r="E9" s="1">
+        <v>14</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="H9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="2"/>
-      <c r="J9" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="K9" s="2"/>
+      <c r="H9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -955,7 +967,6 @@
     <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
update PLM Iteration LOC
Reflex LOC for developing back-end services
</commit_message>
<xml_diff>
--- a/documentation/codeAnalysis/PLM-iteration1-evaluation.xlsx
+++ b/documentation/codeAnalysis/PLM-iteration1-evaluation.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14440" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14260" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="iteration1" sheetId="1" r:id="rId1"/>
@@ -669,7 +669,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I10" sqref="I10"/>
+      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -756,8 +756,8 @@
         <v>0</v>
       </c>
       <c r="C4" s="1">
-        <f xml:space="preserve"> 136 + 46</f>
-        <v>182</v>
+        <f xml:space="preserve"> 136 + 46 + 350</f>
+        <v>532</v>
       </c>
       <c r="D4" s="1">
         <f xml:space="preserve"> 0 + 3</f>
@@ -791,15 +791,15 @@
         <v>14</v>
       </c>
       <c r="C5" s="1">
-        <f xml:space="preserve"> 137 + 60</f>
-        <v>197</v>
+        <f xml:space="preserve"> 137 + 60 + 350</f>
+        <v>547</v>
       </c>
       <c r="D5" s="1">
         <f xml:space="preserve"> 0 + 3</f>
         <v>3</v>
       </c>
       <c r="E5" s="1">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="F5" s="1">
         <v>0</v>
@@ -826,8 +826,8 @@
         <v>15</v>
       </c>
       <c r="C6" s="1">
-        <f xml:space="preserve"> 184 + 3</f>
-        <v>187</v>
+        <f xml:space="preserve"> 184 + 3 + 350</f>
+        <v>537</v>
       </c>
       <c r="D6" s="1">
         <f xml:space="preserve"> 0 + 1</f>
@@ -861,15 +861,15 @@
         <v>16</v>
       </c>
       <c r="C7" s="1">
-        <f xml:space="preserve"> 137 +  225</f>
-        <v>362</v>
+        <f xml:space="preserve"> 137 +  225 + 350</f>
+        <v>712</v>
       </c>
       <c r="D7" s="1">
         <f xml:space="preserve"> 0  + 5</f>
         <v>5</v>
       </c>
       <c r="E7" s="1">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="F7" s="1">
         <v>0</v>
@@ -896,15 +896,15 @@
         <v>17</v>
       </c>
       <c r="C8" s="1">
-        <f xml:space="preserve"> 149 + 239</f>
-        <v>388</v>
+        <f xml:space="preserve"> 149 + 239 + 350</f>
+        <v>738</v>
       </c>
       <c r="D8" s="1">
         <f xml:space="preserve"> 0 + 8</f>
         <v>8</v>
       </c>
       <c r="E8" s="1">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F8" s="1">
         <v>0</v>
@@ -939,7 +939,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="1">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>

</xml_diff>